<commit_message>
split BF improvements between BF and CF; fix target pop for BF and CF; rename MMN to Antenatal MN; remove Proph Zinc Supp
</commit_message>
<xml_diff>
--- a/input_spreadsheets/Bangladesh/2016Oct/subregionSpreadsheets/Barisal.xlsx
+++ b/input_spreadsheets/Bangladesh/2016Oct/subregionSpreadsheets/Barisal.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-3900" yWindow="-21040" windowWidth="24800" windowHeight="19920" tabRatio="500" firstSheet="3" activeTab="6"/>
+    <workbookView xWindow="-3900" yWindow="-21040" windowWidth="24800" windowHeight="19920" tabRatio="500" firstSheet="18" activeTab="19"/>
   </bookViews>
   <sheets>
     <sheet name="demographics" sheetId="1" r:id="rId1"/>
@@ -314,7 +314,7 @@
     <author>Janka Petravic</author>
   </authors>
   <commentList>
-    <comment ref="D5" authorId="0">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -336,7 +336,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="E5" authorId="0">
+    <comment ref="E4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -358,7 +358,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G7" authorId="0">
+    <comment ref="G6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -385,7 +385,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="323" uniqueCount="80">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="80">
   <si>
     <t>indicators</t>
   </si>
@@ -582,9 +582,6 @@
     <t>Vitamin A supplementation</t>
   </si>
   <si>
-    <t>Multiple micronutrient supplementation</t>
-  </si>
-  <si>
     <t>pregnant women</t>
   </si>
   <si>
@@ -625,6 +622,9 @@
   </si>
   <si>
     <t>Food security &amp; education</t>
+  </si>
+  <si>
+    <t>Antenatal micronutrient supplementation</t>
   </si>
 </sst>
 </file>
@@ -806,7 +806,7 @@
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="31">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
@@ -829,9 +829,6 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="164" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="4" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="165" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
@@ -842,7 +839,6 @@
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="2" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
@@ -854,6 +850,9 @@
     </xf>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="2" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
   </cellXfs>
   <cellStyles count="69">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
@@ -1495,7 +1494,7 @@
       <c r="A2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="20">
+      <c r="B2" s="19">
         <v>867804.96938603546</v>
       </c>
     </row>
@@ -1503,7 +1502,7 @@
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="20">
+      <c r="B3" s="19">
         <v>177974.0481272742</v>
       </c>
     </row>
@@ -1511,31 +1510,31 @@
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="20">
+      <c r="B4" s="19">
         <v>204555.28420119709</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="B5" s="29">
+        <v>70</v>
+      </c>
+      <c r="B5" s="27">
         <v>0.56799999999999995</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A6" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="B6" s="30">
+        <v>71</v>
+      </c>
+      <c r="B6" s="28">
         <v>0.51200000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="28">
+        <v>72</v>
+      </c>
+      <c r="B7" s="26">
         <v>0.20599999999999999</v>
       </c>
     </row>
@@ -2752,7 +2751,7 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -2812,7 +2811,7 @@
   <sheetData>
     <row r="1" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B1" t="s">
         <v>11</v>
@@ -2920,7 +2919,7 @@
   <dimension ref="A1:F4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -2949,33 +2948,45 @@
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:6" ht="13" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B2" s="29">
+        <v>5.16</v>
+      </c>
+      <c r="C2" s="29">
+        <v>5.16</v>
+      </c>
+      <c r="D2" s="29">
+        <v>1</v>
+      </c>
+      <c r="E2" s="25">
+        <v>1</v>
+      </c>
+      <c r="F2" s="25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A3" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="B2" s="7">
-        <v>5.16</v>
-      </c>
-      <c r="C2" s="7">
-        <v>5.16</v>
-      </c>
-      <c r="D2" s="7">
+      <c r="B3" s="2">
+        <v>1</v>
+      </c>
+      <c r="C3" s="2">
+        <v>1</v>
+      </c>
+      <c r="D3" s="29">
         <v>1.82</v>
       </c>
-      <c r="E2" s="11">
+      <c r="E3" s="25">
         <v>1.82</v>
       </c>
-      <c r="F2" s="12">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
+      <c r="F3" s="2">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2"/>
@@ -3080,7 +3091,7 @@
       <c r="A2" s="5">
         <v>2017</v>
       </c>
-      <c r="B2" s="15">
+      <c r="B2" s="14">
         <v>176353.82451576061</v>
       </c>
     </row>
@@ -3088,7 +3099,7 @@
       <c r="A3" s="5">
         <v>2018</v>
       </c>
-      <c r="B3" s="15">
+      <c r="B3" s="14">
         <v>174658.49535266697</v>
       </c>
     </row>
@@ -3096,7 +3107,7 @@
       <c r="A4" s="5">
         <v>2019</v>
       </c>
-      <c r="B4" s="15">
+      <c r="B4" s="14">
         <v>172874.16606401838</v>
       </c>
     </row>
@@ -3104,7 +3115,7 @@
       <c r="A5" s="5">
         <v>2020</v>
       </c>
-      <c r="B5" s="15">
+      <c r="B5" s="14">
         <v>170992.31253564314</v>
       </c>
     </row>
@@ -3112,7 +3123,7 @@
       <c r="A6" s="5">
         <v>2021</v>
       </c>
-      <c r="B6" s="15">
+      <c r="B6" s="14">
         <v>169202.0905352431</v>
       </c>
     </row>
@@ -3120,7 +3131,7 @@
       <c r="A7" s="5">
         <v>2022</v>
       </c>
-      <c r="B7" s="15">
+      <c r="B7" s="14">
         <v>167575.14221940024</v>
       </c>
     </row>
@@ -3128,7 +3139,7 @@
       <c r="A8" s="5">
         <v>2023</v>
       </c>
-      <c r="B8" s="15">
+      <c r="B8" s="14">
         <v>165837.38011789907</v>
       </c>
     </row>
@@ -3136,7 +3147,7 @@
       <c r="A9" s="5">
         <v>2024</v>
       </c>
-      <c r="B9" s="15">
+      <c r="B9" s="14">
         <v>163993.39377659772</v>
       </c>
     </row>
@@ -3144,7 +3155,7 @@
       <c r="A10" s="5">
         <v>2025</v>
       </c>
-      <c r="B10" s="15">
+      <c r="B10" s="14">
         <v>162044.77343532885</v>
       </c>
     </row>
@@ -3152,7 +3163,7 @@
       <c r="A11" s="5">
         <v>2026</v>
       </c>
-      <c r="B11" s="15">
+      <c r="B11" s="14">
         <v>159507.77480490523</v>
       </c>
     </row>
@@ -3160,7 +3171,7 @@
       <c r="A12" s="5">
         <v>2027</v>
       </c>
-      <c r="B12" s="15">
+      <c r="B12" s="14">
         <v>157416.57333469548</v>
       </c>
     </row>
@@ -3168,7 +3179,7 @@
       <c r="A13" s="5">
         <v>2028</v>
       </c>
-      <c r="B13" s="15">
+      <c r="B13" s="14">
         <v>155245.66651214968</v>
       </c>
     </row>
@@ -3176,7 +3187,7 @@
       <c r="A14" s="5">
         <v>2029</v>
       </c>
-      <c r="B14" s="15">
+      <c r="B14" s="14">
         <v>152997.78653795182</v>
       </c>
     </row>
@@ -3184,7 +3195,7 @@
       <c r="A15" s="5">
         <v>2030</v>
       </c>
-      <c r="B15" s="15">
+      <c r="B15" s="14">
         <v>150674.07574309639</v>
       </c>
     </row>
@@ -3196,10 +3207,10 @@
 
 <file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G27"/>
+  <dimension ref="A1:G26"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3226,121 +3237,111 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>74</v>
-      </c>
-      <c r="B2" s="23">
-        <v>0</v>
+        <v>64</v>
+      </c>
+      <c r="B2" s="20">
+        <v>0.64100000000000001</v>
       </c>
       <c r="C2" s="2">
         <v>0.85</v>
       </c>
-      <c r="D2" s="21">
-        <v>7.08</v>
+      <c r="D2" s="20">
+        <v>0.35</v>
       </c>
       <c r="E2" s="2"/>
-      <c r="F2" s="13"/>
+      <c r="F2" s="12"/>
       <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B3" s="21">
-        <v>0.64100000000000001</v>
+        <v>75</v>
+      </c>
+      <c r="B3" s="20">
+        <v>0.14000000000000001</v>
       </c>
       <c r="C3" s="2">
         <v>0.85</v>
       </c>
-      <c r="D3" s="21">
-        <v>0.35</v>
+      <c r="D3" s="20">
+        <v>3.56</v>
       </c>
       <c r="E3" s="2"/>
-      <c r="F3" s="13"/>
+      <c r="F3" s="12"/>
       <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" s="2" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="21">
-        <v>0.14000000000000001</v>
+      <c r="B4" s="20">
+        <v>0</v>
       </c>
       <c r="C4" s="2">
         <v>0.85</v>
       </c>
-      <c r="D4" s="21">
-        <v>3.56</v>
+      <c r="D4" s="20">
+        <v>48</v>
       </c>
       <c r="E4" s="2"/>
-      <c r="F4" s="13"/>
+      <c r="F4" s="12"/>
       <c r="G4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
-        <v>77</v>
-      </c>
-      <c r="B5" s="21">
-        <v>0</v>
+        <v>74</v>
+      </c>
+      <c r="B5" s="20">
+        <v>0.61</v>
       </c>
       <c r="C5" s="2">
         <v>0.85</v>
       </c>
-      <c r="D5" s="21">
-        <v>48</v>
+      <c r="D5" s="20">
+        <v>3.56</v>
       </c>
       <c r="E5" s="2"/>
-      <c r="F5" s="13"/>
+      <c r="F5" s="12"/>
       <c r="G5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="21">
-        <v>0.61</v>
+      <c r="A6" t="s">
+        <v>77</v>
+      </c>
+      <c r="B6" s="20">
+        <v>0</v>
       </c>
       <c r="C6" s="2">
         <v>0.85</v>
       </c>
-      <c r="D6" s="21">
-        <v>3.56</v>
+      <c r="D6" s="20">
+        <v>25</v>
       </c>
       <c r="E6" s="2"/>
-      <c r="F6" s="13"/>
+      <c r="F6" s="12"/>
       <c r="G6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>78</v>
-      </c>
-      <c r="B7" s="21">
+        <v>79</v>
+      </c>
+      <c r="B7" s="20">
         <v>0</v>
       </c>
       <c r="C7" s="2">
         <v>0.85</v>
       </c>
-      <c r="D7" s="21">
-        <v>25</v>
+      <c r="D7" s="20">
+        <v>1.81</v>
       </c>
       <c r="E7" s="2"/>
-      <c r="F7" s="13"/>
+      <c r="F7" s="12"/>
       <c r="G7" s="2"/>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="21">
-        <v>0</v>
-      </c>
-      <c r="C8" s="2">
-        <v>0.85</v>
-      </c>
-      <c r="D8" s="21">
-        <v>1.81</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="13"/>
+      <c r="F8" s="2"/>
       <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -3387,10 +3388,7 @@
     </row>
     <row r="15" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2"/>
@@ -3435,10 +3433,6 @@
     <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3447,10 +3441,10 @@
 
 <file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J27"/>
+  <dimension ref="A1:J26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A8"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3483,14 +3477,14 @@
         <v>15</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
     <row r="2" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B2" s="5">
         <v>0</v>
@@ -3499,7 +3493,7 @@
         <v>0</v>
       </c>
       <c r="D2" s="5">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E2" s="5">
         <v>1</v>
@@ -3513,7 +3507,7 @@
     </row>
     <row r="3" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A3" s="2" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="B3" s="5">
         <v>0</v>
@@ -3528,7 +3522,7 @@
         <v>1</v>
       </c>
       <c r="F3" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="G3" s="5">
         <v>0</v>
@@ -3542,13 +3536,15 @@
         <v>0</v>
       </c>
       <c r="C4" s="5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4" s="5">
-        <v>1</v>
+        <f>demographics!$B$6</f>
+        <v>0.51200000000000001</v>
       </c>
       <c r="E4" s="5">
-        <v>1</v>
+        <f>demographics!$B$6</f>
+        <v>0.51200000000000001</v>
       </c>
       <c r="F4" s="5">
         <v>0</v>
@@ -3559,55 +3555,54 @@
     </row>
     <row r="5" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A5" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B5" s="5">
+        <v>1</v>
+      </c>
+      <c r="C5" s="5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="5">
+        <v>0</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0</v>
+      </c>
+      <c r="G5" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>77</v>
       </c>
-      <c r="B5" s="5">
-        <v>0</v>
-      </c>
-      <c r="C5" s="5">
-        <v>0</v>
-      </c>
-      <c r="D5" s="5">
+      <c r="B6" s="5">
+        <v>0</v>
+      </c>
+      <c r="C6" s="5">
+        <v>0</v>
+      </c>
+      <c r="D6" s="5">
+        <v>0</v>
+      </c>
+      <c r="E6" s="5">
+        <v>0</v>
+      </c>
+      <c r="F6" s="5">
+        <v>0</v>
+      </c>
+      <c r="G6" s="5">
         <f>demographics!$B$6</f>
         <v>0.51200000000000001</v>
       </c>
-      <c r="E5" s="5">
-        <f>demographics!$B$6</f>
-        <v>0.51200000000000001</v>
-      </c>
-      <c r="F5" s="5">
-        <v>0</v>
-      </c>
-      <c r="G5" s="5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A6" s="2" t="s">
-        <v>75</v>
-      </c>
-      <c r="B6" s="5">
-        <v>1</v>
-      </c>
-      <c r="C6" s="5">
-        <v>1</v>
-      </c>
-      <c r="D6" s="5">
-        <v>1</v>
-      </c>
-      <c r="E6" s="5">
-        <v>1</v>
-      </c>
-      <c r="F6" s="5">
-        <v>0</v>
-      </c>
-      <c r="G6" s="5">
-        <v>0</v>
-      </c>
     </row>
     <row r="7" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>78</v>
+        <v>79</v>
       </c>
       <c r="B7" s="5">
         <v>0</v>
@@ -3625,32 +3620,15 @@
         <v>0</v>
       </c>
       <c r="G7" s="5">
-        <f>demographics!$B$6</f>
-        <v>0.51200000000000001</v>
+        <v>1</v>
       </c>
     </row>
     <row r="8" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A8" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="B8" s="5">
-        <v>0</v>
-      </c>
-      <c r="C8" s="5">
-        <v>0</v>
-      </c>
-      <c r="D8" s="5">
-        <v>0</v>
-      </c>
-      <c r="E8" s="5">
-        <v>0</v>
-      </c>
-      <c r="F8" s="5">
-        <v>0</v>
-      </c>
-      <c r="G8" s="5">
-        <v>1</v>
-      </c>
+      <c r="B8" s="2"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
     </row>
     <row r="9" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B9" s="2"/>
@@ -3696,10 +3674,7 @@
     </row>
     <row r="15" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
+      <c r="C15" s="2"/>
     </row>
     <row r="16" spans="1:10" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B16" s="2"/>
@@ -3744,10 +3719,6 @@
     <row r="26" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B26" s="2"/>
       <c r="C26" s="2"/>
-    </row>
-    <row r="27" spans="2:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -3761,7 +3732,7 @@
   <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3774,7 +3745,7 @@
         <v>56</v>
       </c>
       <c r="B1" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C1" t="s">
         <v>46</v>
@@ -3791,77 +3762,77 @@
     </row>
     <row r="2" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B2" t="s">
-        <v>68</v>
-      </c>
-      <c r="C2" s="14">
+        <v>67</v>
+      </c>
+      <c r="C2" s="13">
         <v>0.21</v>
       </c>
-      <c r="D2" s="14">
+      <c r="D2" s="13">
         <v>0.21</v>
       </c>
-      <c r="E2" s="14">
-        <v>0</v>
-      </c>
-      <c r="F2" s="14">
+      <c r="E2" s="13">
+        <v>0</v>
+      </c>
+      <c r="F2" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B3" t="s">
-        <v>69</v>
-      </c>
-      <c r="C3" s="14">
-        <f>demographics!$B$5 * 'Interventions target population'!$G$7</f>
+        <v>68</v>
+      </c>
+      <c r="C3" s="13">
+        <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
         <v>0.29081599999999996</v>
       </c>
-      <c r="D3" s="14">
-        <f>demographics!$B$5 * 'Interventions target population'!$G$7</f>
+      <c r="D3" s="13">
+        <f>demographics!$B$5 * 'Interventions target population'!$G$6</f>
         <v>0.29081599999999996</v>
       </c>
-      <c r="E3" s="14">
-        <v>0</v>
-      </c>
-      <c r="F3" s="14">
+      <c r="E3" s="13">
+        <v>0</v>
+      </c>
+      <c r="F3" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>65</v>
+        <v>79</v>
       </c>
       <c r="B4" t="s">
-        <v>68</v>
-      </c>
-      <c r="C4" s="14">
+        <v>67</v>
+      </c>
+      <c r="C4" s="13">
         <v>0.1</v>
       </c>
-      <c r="D4" s="14">
+      <c r="D4" s="13">
         <v>0.1</v>
       </c>
-      <c r="E4" s="14">
-        <v>0</v>
-      </c>
-      <c r="F4" s="14">
+      <c r="E4" s="13">
+        <v>0</v>
+      </c>
+      <c r="F4" s="13">
         <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:6" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B5" t="s">
-        <v>69</v>
-      </c>
-      <c r="C5" s="14">
-        <v>1</v>
-      </c>
-      <c r="D5" s="14">
-        <v>1</v>
-      </c>
-      <c r="E5" s="14">
-        <v>1</v>
-      </c>
-      <c r="F5" s="14">
+        <v>68</v>
+      </c>
+      <c r="C5" s="13">
+        <v>1</v>
+      </c>
+      <c r="D5" s="13">
+        <v>1</v>
+      </c>
+      <c r="E5" s="13">
+        <v>1</v>
+      </c>
+      <c r="F5" s="13">
         <v>0</v>
       </c>
     </row>
@@ -3872,10 +3843,10 @@
 
 <file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="G30" sqref="G30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -3885,7 +3856,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -3908,7 +3879,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
@@ -3920,17 +3891,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
-      </c>
-      <c r="F2" s="27">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="G2" s="27">
-        <v>0.29699999999999999</v>
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="F2" s="25">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="G2" s="25">
+        <v>0.33500000000000002</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
@@ -3943,55 +3913,23 @@
       <c r="E3" s="2">
         <v>0</v>
       </c>
-      <c r="F3" s="27">
-        <v>0.29699999999999999</v>
-      </c>
-      <c r="G3" s="27">
-        <v>0.29699999999999999</v>
+      <c r="F3" s="2">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2">
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="F4" s="27">
-        <v>0.33500000000000002</v>
-      </c>
-      <c r="G4" s="27">
-        <v>0.33500000000000002</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2"/>
@@ -3999,20 +3937,9 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4021,10 +3948,10 @@
 
 <file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A5"/>
+      <selection activeCell="A2" sqref="A2:G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4034,7 +3961,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -4057,7 +3984,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
@@ -4069,17 +3996,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>0.3</v>
       </c>
       <c r="F2" s="2">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
       <c r="G2" s="2">
-        <v>0.5</v>
+        <v>0.3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
@@ -4093,54 +4019,22 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>0.51</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>0.51</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.3</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.3</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2"/>
@@ -4148,20 +4042,9 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4170,10 +4053,10 @@
 
 <file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D22" sqref="D22"/>
+      <selection activeCell="I43" sqref="I43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -4183,7 +4066,7 @@
   <sheetData>
     <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A1" s="2" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>10</v>
@@ -4206,7 +4089,7 @@
     </row>
     <row r="2" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A2" s="2" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>24</v>
@@ -4218,17 +4101,16 @@
         <v>0</v>
       </c>
       <c r="E2" s="2">
-        <v>0</v>
+        <v>0.62</v>
       </c>
       <c r="F2" s="2">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
       <c r="G2" s="2">
-        <v>0.65</v>
+        <v>0.62</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
         <v>25</v>
       </c>
@@ -4242,54 +4124,22 @@
         <v>0</v>
       </c>
       <c r="F3" s="2">
-        <v>0.52</v>
+        <v>0</v>
       </c>
       <c r="G3" s="2">
-        <v>0.52</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A4" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C4" s="2">
-        <v>0</v>
-      </c>
-      <c r="D4" s="2">
-        <v>0</v>
-      </c>
-      <c r="E4" s="2">
-        <v>0.62</v>
-      </c>
-      <c r="F4" s="2">
-        <v>0.62</v>
-      </c>
-      <c r="G4" s="2">
-        <v>0.62</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="C5" s="2">
-        <v>0</v>
-      </c>
-      <c r="D5" s="2">
-        <v>0</v>
-      </c>
-      <c r="E5" s="2">
-        <v>0</v>
-      </c>
-      <c r="F5" s="2">
-        <v>0</v>
-      </c>
-      <c r="G5" s="2">
-        <v>0</v>
-      </c>
+      <c r="A5" s="2"/>
+      <c r="B5" s="2"/>
+      <c r="C5" s="2"/>
+      <c r="D5" s="2"/>
     </row>
     <row r="6" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="B6" s="2"/>
@@ -4297,20 +4147,9 @@
       <c r="D6" s="2"/>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-    </row>
-    <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-    </row>
-    <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -4769,82 +4608,82 @@
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="B2" s="21" t="s">
+      <c r="B2" s="20" t="s">
         <v>36</v>
       </c>
-      <c r="C2" s="24">
+      <c r="C2" s="22">
         <v>49.202001613049148</v>
       </c>
-      <c r="D2" s="24">
+      <c r="D2" s="22">
         <v>49.137521172334814</v>
       </c>
-      <c r="E2" s="24">
+      <c r="E2" s="22">
         <v>37.976948540132589</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="22">
         <v>21.703210571786748</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="22">
         <v>19.610400980935882</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B3" s="21" t="s">
+      <c r="B3" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C3" s="24">
+      <c r="C3" s="22">
         <v>17.518191598342344</v>
       </c>
-      <c r="D3" s="24">
+      <c r="D3" s="22">
         <v>17.495233574730566</v>
       </c>
-      <c r="E3" s="24">
+      <c r="E3" s="22">
         <v>24.307536913563698</v>
       </c>
-      <c r="F3" s="24">
+      <c r="F3" s="22">
         <v>26.245386380069551</v>
       </c>
-      <c r="G3" s="24">
+      <c r="G3" s="22">
         <v>25.703446248327705</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B4" s="21" t="s">
+      <c r="B4" s="20" t="s">
         <v>38</v>
       </c>
-      <c r="C4" s="22">
+      <c r="C4" s="21">
         <v>16.790749718588579</v>
       </c>
-      <c r="D4" s="22">
+      <c r="D4" s="21">
         <v>16.768745025562197</v>
       </c>
-      <c r="E4" s="22">
+      <c r="E4" s="21">
         <v>24.166720772133754</v>
       </c>
-      <c r="F4" s="22">
+      <c r="F4" s="21">
         <v>40.610590962972879</v>
       </c>
-      <c r="G4" s="22">
+      <c r="G4" s="21">
         <v>46.200712795932716</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B5" s="21" t="s">
+      <c r="B5" s="20" t="s">
         <v>39</v>
       </c>
-      <c r="C5" s="22">
+      <c r="C5" s="21">
         <v>3.4362744763058837</v>
       </c>
-      <c r="D5" s="22">
+      <c r="D5" s="21">
         <v>3.431771153567305</v>
       </c>
-      <c r="E5" s="22">
+      <c r="E5" s="21">
         <v>4.4251785927578409</v>
       </c>
-      <c r="F5" s="22">
+      <c r="F5" s="21">
         <v>12.102678252492941</v>
       </c>
-      <c r="G5" s="22">
+      <c r="G5" s="21">
         <v>12.01235975807135</v>
       </c>
     </row>
@@ -4852,82 +4691,82 @@
       <c r="A6" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="B6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="C6" s="26">
+      <c r="C6" s="24">
         <v>52.050561453459785</v>
       </c>
-      <c r="D6" s="26">
+      <c r="D6" s="24">
         <v>51.98234790458136</v>
       </c>
-      <c r="E6" s="26">
+      <c r="E6" s="24">
         <v>53.629675831135003</v>
       </c>
-      <c r="F6" s="26">
+      <c r="F6" s="24">
         <v>50.248357117507744</v>
       </c>
-      <c r="G6" s="26">
+      <c r="G6" s="24">
         <v>44.848260450963195</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B7" s="25" t="s">
+      <c r="B7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="C7" s="26">
+      <c r="C7" s="24">
         <v>21.394071718181319</v>
       </c>
-      <c r="D7" s="26">
+      <c r="D7" s="24">
         <v>21.366034257756201</v>
       </c>
-      <c r="E7" s="26">
+      <c r="E7" s="24">
         <v>21.182634822067307</v>
       </c>
-      <c r="F7" s="26">
+      <c r="F7" s="24">
         <v>27.51257381607083</v>
       </c>
-      <c r="G7" s="26">
+      <c r="G7" s="24">
         <v>35.216094484570654</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B8" s="25" t="s">
+      <c r="B8" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="26">
+      <c r="C8" s="24">
         <v>23.536983019549275</v>
       </c>
-      <c r="D8" s="26">
+      <c r="D8" s="24">
         <v>23.506137220833143</v>
       </c>
-      <c r="E8" s="26">
+      <c r="E8" s="24">
         <v>20.21527800991651</v>
       </c>
-      <c r="F8" s="26">
+      <c r="F8" s="24">
         <v>17.239499766388274</v>
       </c>
-      <c r="G8" s="26">
+      <c r="G8" s="24">
         <v>16.455886140643354</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B9" s="25" t="s">
+      <c r="B9" s="23" t="s">
         <v>39</v>
       </c>
-      <c r="C9" s="26">
+      <c r="C9" s="24">
         <v>6.1620702449346654</v>
       </c>
-      <c r="D9" s="26">
+      <c r="D9" s="24">
         <v>6.1539946993861134</v>
       </c>
-      <c r="E9" s="26">
+      <c r="E9" s="24">
         <v>6.6563616136217139</v>
       </c>
-      <c r="F9" s="26">
+      <c r="F9" s="24">
         <v>5.1497584776131093</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="24">
         <v>2.6376811714603732</v>
       </c>
     </row>
@@ -4938,19 +4777,19 @@
       <c r="B10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="C10" s="16">
+      <c r="C10" s="15">
         <v>80.3</v>
       </c>
-      <c r="D10" s="17">
+      <c r="D10" s="16">
         <v>46.2</v>
       </c>
-      <c r="E10" s="17">
+      <c r="E10" s="16">
         <v>3.3</v>
       </c>
-      <c r="F10" s="17">
+      <c r="F10" s="16">
         <v>0.7</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="18">
         <v>0</v>
       </c>
     </row>
@@ -4958,19 +4797,19 @@
       <c r="B11" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C11" s="16">
+      <c r="C11" s="15">
         <v>6.8</v>
       </c>
-      <c r="D11" s="17">
+      <c r="D11" s="16">
         <v>16.3</v>
       </c>
-      <c r="E11" s="17">
+      <c r="E11" s="16">
         <v>9.4</v>
       </c>
-      <c r="F11" s="17">
+      <c r="F11" s="16">
         <v>4.4000000000000004</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="18">
         <v>0</v>
       </c>
     </row>
@@ -4978,16 +4817,16 @@
       <c r="B12" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="C12" s="16">
+      <c r="C12" s="15">
         <v>10.7</v>
       </c>
-      <c r="D12" s="17">
+      <c r="D12" s="16">
         <v>37.1</v>
       </c>
-      <c r="E12" s="17">
+      <c r="E12" s="16">
         <v>83.7</v>
       </c>
-      <c r="F12" s="17">
+      <c r="F12" s="16">
         <v>87.9</v>
       </c>
       <c r="G12">
@@ -4998,19 +4837,19 @@
       <c r="B13" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C13" s="16">
+      <c r="C13" s="15">
         <v>2.2000000000000002</v>
       </c>
-      <c r="D13" s="17">
+      <c r="D13" s="16">
         <v>0.5</v>
       </c>
-      <c r="E13" s="17">
+      <c r="E13" s="16">
         <v>3.6</v>
       </c>
-      <c r="F13" s="17">
+      <c r="F13" s="16">
         <v>6.9</v>
       </c>
-      <c r="G13" s="18">
+      <c r="G13" s="17">
         <v>100</v>
       </c>
     </row>
@@ -5061,7 +4900,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:F2"/>
     </sheetView>
   </sheetViews>
@@ -5091,19 +4930,19 @@
       <c r="A2" s="2" t="s">
         <v>24</v>
       </c>
-      <c r="B2" s="30">
+      <c r="B2" s="28">
         <v>2.8</v>
       </c>
-      <c r="C2" s="30">
+      <c r="C2" s="28">
         <v>2.8</v>
       </c>
-      <c r="D2" s="30">
+      <c r="D2" s="28">
         <v>4.2699999999999996</v>
       </c>
-      <c r="E2" s="30">
+      <c r="E2" s="28">
         <v>3.46</v>
       </c>
-      <c r="F2" s="30">
+      <c r="F2" s="28">
         <v>2.21</v>
       </c>
     </row>

</xml_diff>